<commit_message>
config file change for docker work
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata - Copy.xlsx
+++ b/src/test/resources/excel/testdata - Copy.xlsx
@@ -436,24 +436,12 @@
     <t>Quick Quote Flow when policy term as 6 months</t>
   </si>
   <si>
-    <t>Quick Quote Flow when user add two Prior Claim under prior claim history tab</t>
-  </si>
-  <si>
-    <t>When State is NJ and company is North River then coverger pricing then NYFTZ is autochecked</t>
-  </si>
-  <si>
     <t>When State is NJ and company is North River then coverger pricing then NJ PLIGA field will be displayed</t>
   </si>
   <si>
-    <t>Rating level is checked for preferred both checked</t>
-  </si>
-  <si>
     <t>Rating level is checked for preferred only</t>
   </si>
   <si>
-    <t>when company is North River verify the schedule rating field validation</t>
-  </si>
-  <si>
     <t>In policy form if print speciman is checked, then list check box will be auto checked</t>
   </si>
   <si>
@@ -470,6 +458,18 @@
   </si>
   <si>
     <t>The North River Insurance Company</t>
+  </si>
+  <si>
+    <t>Quick Quote Flow when user adds two Prior Claim under prior claim history tab</t>
+  </si>
+  <si>
+    <t>When State is NY and company is North River then NYFTZ is autochecked</t>
+  </si>
+  <si>
+    <t>Rating level is checked for standard and preferred both checked</t>
+  </si>
+  <si>
+    <t>when company is North River verify the schedule rating field validation -state specific ????? DCP-7786</t>
   </si>
 </sst>
 </file>
@@ -860,7 +860,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,7 +918,7 @@
         <v>127</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>2</v>
@@ -929,7 +929,7 @@
         <v>128</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -940,7 +940,7 @@
         <v>129</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>2</v>
@@ -951,7 +951,7 @@
         <v>130</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>2</v>
@@ -962,7 +962,7 @@
         <v>131</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>2</v>
@@ -973,7 +973,7 @@
         <v>132</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>2</v>
@@ -984,7 +984,7 @@
         <v>133</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>2</v>
@@ -1111,7 +1111,7 @@
         <v>23</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>123</v>
@@ -1350,7 +1350,7 @@
         <v>34</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="W2" s="5" t="s">
         <v>40</v>
@@ -1595,7 +1595,7 @@
         <v>34</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="W3" s="5" t="s">
         <v>40</v>
@@ -2043,7 +2043,7 @@
         <v>36</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>37</v>
@@ -2094,7 +2094,7 @@
         <v>28</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="Z5" s="3" t="s">
         <v>64</v>

</xml_diff>